<commit_message>
send email attachments (last)
</commit_message>
<xml_diff>
--- a/Task1(v4)/pridetiDT.xlsx
+++ b/Task1(v4)/pridetiDT.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9315" xr2:uid="{0A2E20A7-206E-4489-BC20-AE5859AFB31A}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="9315" xr2:uid="{BDCC92BE-6791-4BD2-8F37-D90E88C85154}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -380,7 +380,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F201008-8B7A-4C05-94B6-A20B2EE60CDA}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B7D7E2E-38BE-4A1C-9210-1CDC878EF55E}">
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>

</xml_diff>